<commit_message>
Modified stuff - optimal is broken or something
</commit_message>
<xml_diff>
--- a/data/algorithm_performance/comparison.xlsx
+++ b/data/algorithm_performance/comparison.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Documents\Cloned Repos\mthe_493\data\algorithm_performance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{1EAD5AC5-F3B4-41CE-86B5-D117A97C1DA4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C15759BF-5C91-4AC2-9558-7FFF98F2F2B4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="21520" windowHeight="11586"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="21520" windowHeight="11586" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ipopt" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2293,11 +2293,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>

</xml_diff>